<commit_message>
Update on 20200407 part 2
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200402/配合固网华为vIMS网络建设，请进行业务开通、资源、计费等方面的开发（195665795）/配合固网华为vIMS网络建设，请进行业务开通、资源、计费等方面的开发（195665795）测试报告.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200402/配合固网华为vIMS网络建设，请进行业务开通、资源、计费等方面的开发（195665795）/配合固网华为vIMS网络建设，请进行业务开通、资源、计费等方面的开发（195665795）测试报告.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t>序号</t>
   </si>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>张轶晟</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>需求提出部门</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -320,18 +316,6 @@
         <charset val="134"/>
       </rPr>
       <t>固定电话普通接入新装</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>张轶晟</t>
     </r>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -862,6 +846,15 @@
     <xf numFmtId="176" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -869,15 +862,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1155,7 +1139,7 @@
   <dimension ref="A1:IT16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1203,7 +1187,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -1215,19 +1199,19 @@
         <v>12</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>15</v>
@@ -1475,53 +1459,51 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="18"/>
-      <c r="F2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="21">
+        <v>12</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="24">
+        <v>195665795</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="24">
-        <v>12</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="21">
-        <v>195665795</v>
-      </c>
-      <c r="M2" s="21" t="s">
+      <c r="O2" s="24"/>
+      <c r="P2" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="24">
+        <v>20200414</v>
+      </c>
+      <c r="S2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="21">
-        <v>20200414</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="21"/>
+      <c r="T2" s="24"/>
       <c r="U2" s="15"/>
       <c r="V2" s="15"/>
       <c r="W2" s="15"/>
@@ -1765,27 +1747,27 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" s="18"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
       <c r="U3" s="15"/>
       <c r="V3" s="15"/>
       <c r="W3" s="15"/>
@@ -2029,27 +2011,27 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
     </row>
     <row r="5" spans="1:254" ht="36">
       <c r="A5" s="13">
@@ -2059,27 +2041,27 @@
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:254" ht="24">
       <c r="A6" s="13">
@@ -2089,27 +2071,27 @@
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:254" ht="24">
       <c r="A7" s="13">
@@ -2119,27 +2101,27 @@
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
     </row>
     <row r="8" spans="1:254" ht="24">
       <c r="A8" s="13">
@@ -2149,27 +2131,27 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
     </row>
     <row r="9" spans="1:254" ht="24">
       <c r="A9" s="13">
@@ -2179,27 +2161,27 @@
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
     </row>
     <row r="10" spans="1:254" ht="48">
       <c r="A10" s="13">
@@ -2209,27 +2191,27 @@
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
     </row>
     <row r="11" spans="1:254" ht="48">
       <c r="A11" s="13">
@@ -2239,27 +2221,27 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
     </row>
     <row r="12" spans="1:254" ht="36">
       <c r="A12" s="13">
@@ -2269,27 +2251,27 @@
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
     </row>
     <row r="13" spans="1:254" ht="36">
       <c r="A13" s="13">
@@ -2299,33 +2281,38 @@
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
     </row>
     <row r="16" spans="1:254">
       <c r="D16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="P2:P13"/>
+    <mergeCell ref="Q2:Q13"/>
+    <mergeCell ref="R2:R13"/>
+    <mergeCell ref="S2:S13"/>
+    <mergeCell ref="T2:T13"/>
     <mergeCell ref="F2:F13"/>
     <mergeCell ref="G2:G13"/>
     <mergeCell ref="I2:I13"/>
@@ -2336,11 +2323,6 @@
     <mergeCell ref="L2:L13"/>
     <mergeCell ref="M2:M13"/>
     <mergeCell ref="N2:N13"/>
-    <mergeCell ref="P2:P13"/>
-    <mergeCell ref="Q2:Q13"/>
-    <mergeCell ref="R2:R13"/>
-    <mergeCell ref="S2:S13"/>
-    <mergeCell ref="T2:T13"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2352,7 +2334,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -2373,25 +2355,25 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>17</v>
@@ -2400,7 +2382,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>18</v>
@@ -2411,32 +2393,30 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="20">
         <v>43923</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="20">
         <v>43923.6875</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="24.75">
@@ -2444,32 +2424,30 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="20">
         <v>43923</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="20">
         <v>43923.6875</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="24.75">
@@ -2477,32 +2455,30 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="20">
         <v>43923</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="20">
         <v>43923.6875</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.5">
@@ -2510,32 +2486,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="20">
         <v>43923.625</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="20">
         <v>43924.4375</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="24">
@@ -2543,32 +2517,30 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="20">
         <v>43923.625</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="20">
         <v>43924.4375</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11">

</xml_diff>